<commit_message>
Dimension 2  limpias y en app
</commit_message>
<xml_diff>
--- a/data/raw/plan_Con_Pre_100522.xlsx
+++ b/data/raw/plan_Con_Pre_100522.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="312">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -1232,20 +1232,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ98"/>
+  <dimension ref="A1:AMD98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AMA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="AMA1" activeCellId="0" sqref="AMA1"/>
+      <selection pane="bottomLeft" activeCell="T1" activeCellId="0" sqref="T1:AMJ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="1" style="0" width="18.88"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1303,3021 +1303,165 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AW1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BG1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="BH1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="BK1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="BL1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="BM1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="BO1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="BP1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="BW1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BZ1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="CA1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="CF1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="CG1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="CH1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="CI1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="CJ1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="CK1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="CL1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="CM1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="CN1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="CO1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="CP1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="CQ1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="CR1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="CS1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="CT1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="CU1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="CV1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="CW1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="CX1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="CY1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="CZ1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="DA1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="DB1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="DC1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DD1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="DE1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="DF1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="DG1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="DH1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="DI1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="DL1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="DM1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="DN1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="DO1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="DP1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="DQ1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="DR1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="DS1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="DT1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="DU1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="DV1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="DW1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="DX1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="DY1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="DZ1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="EA1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="EB1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="EC1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="ED1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="EE1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="EF1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="EG1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="EH1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="EI1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="EJ1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="EK1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="EL1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="EM1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="EN1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="EO1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EP1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="EQ1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="ER1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="ES1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="ET1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="EU1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="EV1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="EW1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="EX1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="EY1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="EZ1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="FA1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="FB1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="FC1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="FD1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="FE1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="FF1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="FG1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="FH1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="FI1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="FJ1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="FK1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="FL1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="FM1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="FN1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="FO1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="FP1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="FQ1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="FR1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="FS1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="FT1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="FU1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="FV1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="FW1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="FX1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="FY1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="FZ1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="GA1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GB1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="GC1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="GD1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="GE1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="GF1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="GG1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="GH1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="GI1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="GJ1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="GK1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="GL1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="GM1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="GN1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="GO1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="GP1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="GQ1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="GR1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="GS1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="GT1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="GU1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="GV1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="GW1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="GX1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="GY1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="GZ1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="HA1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="HB1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="HC1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="HD1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="HE1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="HF1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="HG1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="HH1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="HI1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="HJ1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="HK1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="HL1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="HM1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="HN1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="HO1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="HP1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="HQ1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="HR1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="HS1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="HT1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="HU1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="HV1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="HW1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="HX1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="HY1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="HZ1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="IA1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="IB1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="IC1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="ID1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="IE1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="IF1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="IG1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="IH1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="II1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="IJ1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="IK1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="IL1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="IM1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="IN1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="IO1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="IP1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="IQ1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="IR1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="IS1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="IT1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="IU1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="IV1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="IW1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="IX1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="IY1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="IZ1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="JA1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="JB1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="JC1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="JD1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="JE1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="JF1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="JG1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="JH1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="JI1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="JJ1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="JK1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="JL1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="JM1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="JN1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="JO1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="JP1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="JQ1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="JR1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="JS1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="JT1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="JU1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="JV1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="JW1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="JX1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="JY1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="JZ1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="KA1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="KB1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="KC1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="KD1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="KE1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="KF1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="KG1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="KH1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="KI1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="KJ1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="KK1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="KL1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="KM1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="KN1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="KO1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="KP1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="KQ1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="KR1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="KS1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="KT1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="KU1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="KV1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="KW1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="KX1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="KY1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="KZ1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="LA1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="LB1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="LC1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="LD1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="LE1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="LF1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="LG1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="LH1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="LI1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="LJ1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="LK1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="LL1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="LM1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="LN1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="LO1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="LP1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="LQ1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="LR1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="LS1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="LT1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="LU1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="LV1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="LW1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="LX1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="LY1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="LZ1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="MA1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="MB1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="MC1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="MD1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="ME1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="MF1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="MG1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="MH1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="MI1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="MJ1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="MK1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="ML1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="MM1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="MN1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="MO1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="MP1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="MQ1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="MR1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="MS1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="MT1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="MU1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="MV1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="MW1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="MX1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="MY1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="MZ1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="NA1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="NB1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="NC1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="ND1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="NE1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="NF1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="NG1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="NH1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="NI1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="NJ1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="NK1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="NL1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="NM1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="NN1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="NO1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="NP1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="NQ1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="NR1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="NS1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="NT1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="NU1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="NV1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="NW1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="NX1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="NY1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="NZ1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="OA1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="OB1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="OC1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="OD1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="OE1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="OF1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="OG1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="OH1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="OI1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="OJ1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="OK1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="OL1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="OM1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="ON1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="OO1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="OP1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="OQ1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="OR1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="OS1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="OT1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="OU1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="OV1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="OW1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="OX1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="OY1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="OZ1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="PA1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="PB1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="PC1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="PD1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="PE1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="PF1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="PG1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="PH1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="PI1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="PJ1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="PK1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="PL1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="PM1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="PN1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="PO1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="PP1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="PQ1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="PR1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="PS1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="PT1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="PU1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="PV1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="PW1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="PX1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="PY1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="PZ1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="QA1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="QB1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="QC1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="QD1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="QE1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="QF1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="QG1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="QH1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="QI1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="QJ1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="QK1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="QL1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="QM1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="QN1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="QO1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="QP1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="QQ1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="QR1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="QS1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="QT1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="QU1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="QV1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="QW1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="QX1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="QY1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="QZ1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="RA1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="RB1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="RC1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="RD1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="RE1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="RF1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="RG1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="RH1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="RI1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="RJ1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="RK1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="RL1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="RM1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="RN1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="RO1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="RP1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="RQ1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="RR1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="RS1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="RT1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="RU1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="RV1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="RW1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="RX1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="RY1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="RZ1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="SA1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="SB1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="SC1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="SD1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="SE1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="SF1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="SG1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="SH1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="SI1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="SJ1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="SK1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="SL1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="SM1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="SN1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="SO1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="SP1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="SQ1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="SR1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="SS1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="ST1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="SU1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="SV1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="SW1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="SX1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="SY1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="SZ1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="TA1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="TB1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="TC1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="TD1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="TE1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="TF1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="TG1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="TH1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="TI1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="TJ1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="TK1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="TL1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="TM1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="TN1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="TO1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="TP1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="TQ1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="TR1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="TS1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="TT1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="TU1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="TV1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="TW1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="TX1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="TY1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="TZ1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="UA1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="UB1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="UC1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="UD1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="UE1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="UF1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="UG1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="UH1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="UI1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="UJ1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="UK1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="UL1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="UM1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="UN1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="UO1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="UP1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="UQ1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="UR1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="US1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="UT1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="UU1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="UV1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="UW1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="UX1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="UY1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="UZ1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="VA1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="VB1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="VC1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="VD1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="VE1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="VF1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="VG1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="VH1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="VI1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="VJ1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="VK1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="VL1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="VM1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="VN1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="VO1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="VP1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="VQ1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="VR1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="VS1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="VT1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="VU1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="VV1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="VW1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="VX1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="VY1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="VZ1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="WA1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="WB1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="WC1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="WD1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="WE1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="WF1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="WG1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="WH1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="WI1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="WJ1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="WK1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="WL1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="WM1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="WN1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="WO1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="WP1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="WQ1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="WR1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="WS1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="WT1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="WU1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="WV1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="WW1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="WX1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="WY1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="WZ1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="XA1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="XB1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="XC1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="XD1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="XE1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="XF1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="XG1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="XH1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="XI1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="XJ1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="XK1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="XL1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="XM1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="XN1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="XO1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="XP1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="XQ1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="XR1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="XS1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="XT1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="XU1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="XV1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="XW1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="XX1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="XY1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="XZ1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="YA1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="YB1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="YC1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="YD1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="YE1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="YF1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="YG1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="YH1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="YI1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="YJ1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="YK1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="YL1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="YM1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="YN1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="YO1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="YP1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="YQ1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="YR1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="YS1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="YT1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="YU1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="YV1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="YW1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="YX1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="YY1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="YZ1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="ZA1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ZB1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="ZC1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="ZD1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="ZE1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="ZF1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="ZG1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="ZH1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="ZI1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="ZJ1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="ZK1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="ZL1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="ZM1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="ZN1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="ZO1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="ZP1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="ZQ1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="ZR1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="ZS1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="ZT1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ZU1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="ZV1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="ZW1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="ZX1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="ZY1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="ZZ1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AAA1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AAB1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AAC1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AAD1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AAE1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AAF1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AAG1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AAH1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AAI1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AAJ1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AAK1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AAL1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AAM1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AAN1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AAO1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AAP1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AAQ1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AAR1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AAS1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AAT1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AAU1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AAV1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AAW1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AAX1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AAY1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AAZ1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="ABA1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="ABB1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="ABC1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="ABD1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="ABE1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="ABF1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ABG1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="ABH1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="ABI1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="ABJ1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="ABK1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="ABL1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="ABM1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="ABN1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="ABO1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="ABP1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="ABQ1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="ABR1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="ABS1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="ABT1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="ABU1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="ABV1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="ABW1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="ABX1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="ABY1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ABZ1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="ACA1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="ACB1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="ACC1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="ACD1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="ACE1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="ACF1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="ACG1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="ACH1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="ACI1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="ACJ1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="ACK1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="ACL1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="ACM1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="ACN1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="ACO1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="ACP1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="ACQ1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="ACR1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ACS1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="ACT1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="ACU1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="ACV1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="ACW1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="ACX1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="ACY1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="ACZ1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="ADA1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="ADB1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="ADC1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="ADD1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="ADE1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="ADF1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="ADG1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="ADH1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="ADI1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="ADJ1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="ADK1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ADL1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="ADM1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="ADN1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="ADO1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="ADP1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="ADQ1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="ADR1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="ADS1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="ADT1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="ADU1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="ADV1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="ADW1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="ADX1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="ADY1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="ADZ1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AEA1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AEB1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AEC1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AED1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AEE1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AEF1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AEG1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AEH1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AEI1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AEJ1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AEK1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AEL1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AEM1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AEN1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AEO1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AEP1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AEQ1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AER1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AES1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AET1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AEU1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AEV1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AEW1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AEX1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AEY1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AEZ1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AFA1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AFB1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AFC1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AFD1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AFE1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AFF1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AFG1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AFH1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AFI1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AFJ1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AFK1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AFL1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AFM1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AFN1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AFO1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AFP1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AFQ1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AFR1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AFS1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AFT1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AFU1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AFV1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AFW1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AFX1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AFY1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AFZ1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AGA1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AGB1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AGC1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AGD1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AGE1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AGF1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AGG1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AGH1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AGI1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AGJ1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AGK1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AGL1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AGM1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AGN1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AGO1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AGP1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AGQ1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AGR1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AGS1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AGT1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AGU1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AGV1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AGW1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AGX1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AGY1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AGZ1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AHA1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AHB1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AHC1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AHD1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AHE1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AHF1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AHG1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AHH1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AHI1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AHJ1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AHK1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AHL1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AHM1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AHN1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AHO1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AHP1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AHQ1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AHR1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AHS1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AHT1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AHU1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AHV1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AHW1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AHX1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AHY1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AHZ1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AIA1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AIB1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AIC1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AID1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AIE1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AIF1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AIG1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AIH1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AII1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AIJ1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AIK1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AIL1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AIM1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AIN1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AIO1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AIP1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AIQ1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AIR1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AIS1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AIT1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AIU1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AIV1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AIW1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AIX1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AIY1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AIZ1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJA1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJB1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJC1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AJD1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJE1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJF1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJG1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJH1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJI1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJJ1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AJK1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJL1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJM1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJN1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJO1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJP1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJQ1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJR1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJS1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJT1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJU1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJV1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AJW1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJX1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJY1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJZ1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AKA1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AKB1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AKC1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AKD1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AKE1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AKF1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AKG1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AKH1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AKI1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AKJ1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AKK1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AKL1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AKM1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AKN1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AKO1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AKP1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AKQ1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AKR1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AKS1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AKT1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AKU1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AKV1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AKW1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AKX1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AKY1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AKZ1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="ALA1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="ALB1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="ALC1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="ALD1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="ALE1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="ALF1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="ALG1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="ALH1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="ALI1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="ALJ1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="ALK1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="ALL1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="ALM1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="ALN1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="ALO1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="ALP1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="ALQ1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="ALR1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="ALS1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="ALT1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="ALU1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="ALV1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="ALW1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="ALX1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="ALY1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="ALZ1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AMA1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AMB1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AMC1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AMD1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AME1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AMF1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AMG1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AMH1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AMI1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AMJ1" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="U1" s="2"/>
+      <c r="V1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="3"/>
+      <c r="AW1" s="3"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="3"/>
+      <c r="BP1" s="3"/>
+      <c r="BZ1" s="2"/>
+      <c r="CA1" s="3"/>
+      <c r="CI1" s="3"/>
+      <c r="CS1" s="2"/>
+      <c r="CT1" s="3"/>
+      <c r="DB1" s="3"/>
+      <c r="DL1" s="2"/>
+      <c r="DM1" s="3"/>
+      <c r="DU1" s="3"/>
+      <c r="EE1" s="2"/>
+      <c r="EF1" s="3"/>
+      <c r="EN1" s="3"/>
+      <c r="EX1" s="2"/>
+      <c r="EY1" s="3"/>
+      <c r="FG1" s="3"/>
+      <c r="FQ1" s="2"/>
+      <c r="FR1" s="3"/>
+      <c r="FZ1" s="3"/>
+      <c r="GJ1" s="2"/>
+      <c r="GK1" s="3"/>
+      <c r="GS1" s="3"/>
+      <c r="HC1" s="2"/>
+      <c r="HD1" s="3"/>
+      <c r="HL1" s="3"/>
+      <c r="HV1" s="2"/>
+      <c r="HW1" s="3"/>
+      <c r="IE1" s="3"/>
+      <c r="IO1" s="2"/>
+      <c r="IP1" s="3"/>
+      <c r="IX1" s="3"/>
+      <c r="JH1" s="2"/>
+      <c r="JI1" s="3"/>
+      <c r="JQ1" s="3"/>
+      <c r="KA1" s="2"/>
+      <c r="KB1" s="3"/>
+      <c r="KJ1" s="3"/>
+      <c r="KT1" s="2"/>
+      <c r="KU1" s="3"/>
+      <c r="LC1" s="3"/>
+      <c r="LM1" s="2"/>
+      <c r="LN1" s="3"/>
+      <c r="LV1" s="3"/>
+      <c r="MF1" s="2"/>
+      <c r="MG1" s="3"/>
+      <c r="MO1" s="3"/>
+      <c r="MY1" s="2"/>
+      <c r="MZ1" s="3"/>
+      <c r="NH1" s="3"/>
+      <c r="NR1" s="2"/>
+      <c r="NS1" s="3"/>
+      <c r="OA1" s="3"/>
+      <c r="OK1" s="2"/>
+      <c r="OL1" s="3"/>
+      <c r="OT1" s="3"/>
+      <c r="PD1" s="2"/>
+      <c r="PE1" s="3"/>
+      <c r="PM1" s="3"/>
+      <c r="PW1" s="2"/>
+      <c r="PX1" s="3"/>
+      <c r="QF1" s="3"/>
+      <c r="QP1" s="2"/>
+      <c r="QQ1" s="3"/>
+      <c r="QY1" s="3"/>
+      <c r="RI1" s="2"/>
+      <c r="RJ1" s="3"/>
+      <c r="RR1" s="3"/>
+      <c r="SB1" s="2"/>
+      <c r="SC1" s="3"/>
+      <c r="SK1" s="3"/>
+      <c r="SU1" s="2"/>
+      <c r="SV1" s="3"/>
+      <c r="TD1" s="3"/>
+      <c r="TN1" s="2"/>
+      <c r="TO1" s="3"/>
+      <c r="TW1" s="3"/>
+      <c r="UG1" s="2"/>
+      <c r="UH1" s="3"/>
+      <c r="UP1" s="3"/>
+      <c r="UZ1" s="2"/>
+      <c r="VA1" s="3"/>
+      <c r="VI1" s="3"/>
+      <c r="VS1" s="2"/>
+      <c r="VT1" s="3"/>
+      <c r="WB1" s="3"/>
+      <c r="WL1" s="2"/>
+      <c r="WM1" s="3"/>
+      <c r="WU1" s="3"/>
+      <c r="XE1" s="2"/>
+      <c r="XF1" s="3"/>
+      <c r="XN1" s="3"/>
+      <c r="XX1" s="2"/>
+      <c r="XY1" s="3"/>
+      <c r="YG1" s="3"/>
+      <c r="YQ1" s="2"/>
+      <c r="YR1" s="3"/>
+      <c r="YZ1" s="3"/>
+      <c r="ZJ1" s="2"/>
+      <c r="ZK1" s="3"/>
+      <c r="ZS1" s="3"/>
+      <c r="AAC1" s="2"/>
+      <c r="AAD1" s="3"/>
+      <c r="AAL1" s="3"/>
+      <c r="AAV1" s="2"/>
+      <c r="AAW1" s="3"/>
+      <c r="ABE1" s="3"/>
+      <c r="ABO1" s="2"/>
+      <c r="ABP1" s="3"/>
+      <c r="ABX1" s="3"/>
+      <c r="ACH1" s="2"/>
+      <c r="ACI1" s="3"/>
+      <c r="ACQ1" s="3"/>
+      <c r="ADA1" s="2"/>
+      <c r="ADB1" s="3"/>
+      <c r="ADJ1" s="3"/>
+      <c r="ADT1" s="2"/>
+      <c r="ADU1" s="3"/>
+      <c r="AEC1" s="3"/>
+      <c r="AEM1" s="2"/>
+      <c r="AEN1" s="3"/>
+      <c r="AEV1" s="3"/>
+      <c r="AFF1" s="2"/>
+      <c r="AFG1" s="3"/>
+      <c r="AFO1" s="3"/>
+      <c r="AFY1" s="2"/>
+      <c r="AFZ1" s="3"/>
+      <c r="AGH1" s="3"/>
+      <c r="AGR1" s="2"/>
+      <c r="AGS1" s="3"/>
+      <c r="AHA1" s="3"/>
+      <c r="AHK1" s="2"/>
+      <c r="AHL1" s="3"/>
+      <c r="AHT1" s="3"/>
+      <c r="AID1" s="2"/>
+      <c r="AIE1" s="3"/>
+      <c r="AIM1" s="3"/>
+      <c r="AIW1" s="2"/>
+      <c r="AIX1" s="3"/>
+      <c r="AJF1" s="3"/>
+      <c r="AJP1" s="2"/>
+      <c r="AJQ1" s="3"/>
+      <c r="AJY1" s="3"/>
+      <c r="AKI1" s="2"/>
+      <c r="AKJ1" s="3"/>
+      <c r="AKR1" s="3"/>
+      <c r="ALB1" s="2"/>
+      <c r="ALC1" s="3"/>
+      <c r="ALK1" s="3"/>
+      <c r="ALU1" s="2"/>
+      <c r="ALV1" s="3"/>
+      <c r="AMD1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">

</xml_diff>